<commit_message>
fixed indentation issue and data_type issue  in calc_bioreactor, elaborated error statements
</commit_message>
<xml_diff>
--- a/Bioreaktor_forPy.xlsx
+++ b/Bioreaktor_forPy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Server\Tools\python\FermentALADIN\FermentationModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024EC097-95CA-4C09-9C51-B6AA5B8FD9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1EDA59A-AC00-42DD-8E65-D7ADD7016D49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E3D132-4FA8-40D7-B6AE-50FDCDDD87B9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{66E3D132-4FA8-40D7-B6AE-50FDCDDD87B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hübsch" sheetId="5" r:id="rId1"/>
@@ -950,6 +950,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -961,9 +964,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2220,32 +2220,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1D0311-A791-4A82-9479-DEE4F4685D3B}">
   <dimension ref="A1:AD39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15:R17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" outlineLevelRow="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.69140625" customWidth="1"/>
+    <col min="2" max="2" width="13.15234375" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.3828125" customWidth="1"/>
+    <col min="5" max="5" width="15.3828125" customWidth="1"/>
+    <col min="6" max="6" width="7.3828125" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="4.42578125" customWidth="1"/>
-    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="4.3828125" customWidth="1"/>
+    <col min="9" max="9" width="3.69140625" customWidth="1"/>
     <col min="10" max="10" width="3" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="5.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="5.69140625" customWidth="1"/>
+    <col min="12" max="12" width="9.3046875" customWidth="1"/>
+    <col min="13" max="13" width="11.3828125" customWidth="1"/>
+    <col min="14" max="14" width="5.3828125" customWidth="1"/>
+    <col min="15" max="15" width="9.3046875" customWidth="1"/>
+    <col min="16" max="16" width="7.69140625" customWidth="1"/>
+    <col min="18" max="18" width="16.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:30" ht="23.6" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A1" s="40"/>
       <c r="B1" s="41" t="s">
         <v>38</v>
@@ -2281,7 +2281,7 @@
       <c r="AC1" s="40"/>
       <c r="AD1" s="40"/>
     </row>
-    <row r="2" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="40"/>
       <c r="B2" s="56" t="s">
         <v>41</v>
@@ -2327,16 +2327,16 @@
       <c r="AC2" s="40"/>
       <c r="AD2" s="40"/>
     </row>
-    <row r="3" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A3" s="40"/>
       <c r="B3" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="65" t="str">
+      <c r="C3" s="66" t="str">
         <f>VLOOKUP($C$2,ModelDB[],3,FALSE)</f>
         <v>S.cerevisiae</v>
       </c>
-      <c r="D3" s="65"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
@@ -2349,17 +2349,13 @@
         <v>40</v>
       </c>
       <c r="N3" s="39">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="O3" s="61">
-        <v>10</v>
-      </c>
-      <c r="P3" s="62">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="39">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="P3" s="62"/>
+      <c r="Q3" s="39"/>
       <c r="R3" s="29"/>
       <c r="S3" s="28"/>
       <c r="T3" s="28"/>
@@ -2376,7 +2372,7 @@
       <c r="AC3" s="40"/>
       <c r="AD3" s="40"/>
     </row>
-    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="40"/>
       <c r="B4" s="40"/>
       <c r="C4" s="40"/>
@@ -2389,14 +2385,14 @@
       <c r="J4" s="40"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
-      <c r="M4" s="66" t="s">
+      <c r="M4" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="69"/>
       <c r="S4" s="28"/>
       <c r="T4" s="28"/>
       <c r="U4" s="28"/>
@@ -2410,7 +2406,7 @@
       <c r="AC4" s="40"/>
       <c r="AD4" s="40"/>
     </row>
-    <row r="5" spans="1:30" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="40"/>
       <c r="B5" s="45" t="s">
         <v>31</v>
@@ -2456,7 +2452,7 @@
       <c r="AC5" s="40"/>
       <c r="AD5" s="40"/>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A6" s="40"/>
       <c r="C6" s="15">
         <v>0</v>
@@ -2493,20 +2489,20 @@
       <c r="AC6" s="40"/>
       <c r="AD6" s="40"/>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A7" s="40"/>
       <c r="B7" s="40"/>
       <c r="C7" s="15">
         <f>C6+$N$3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D7" s="37">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E7" s="40"/>
       <c r="F7" s="15">
         <f>F6+$N$3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G7" s="37">
         <v>1000</v>
@@ -2535,24 +2531,20 @@
       <c r="AC7" s="40"/>
       <c r="AD7" s="40"/>
     </row>
-    <row r="8" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="A8" s="40"/>
       <c r="B8" s="40"/>
       <c r="C8" s="15">
         <f>C7+$O$3</f>
-        <v>20</v>
-      </c>
-      <c r="D8" s="37">
-        <v>0.2</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D8" s="37"/>
       <c r="E8" s="40"/>
       <c r="F8" s="15">
         <f>F7+$O$3</f>
-        <v>20</v>
-      </c>
-      <c r="G8" s="37">
-        <v>1200</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G8" s="37"/>
       <c r="H8" s="40"/>
       <c r="I8" s="40"/>
       <c r="J8" s="40"/>
@@ -2577,24 +2569,20 @@
       <c r="AC8" s="40"/>
       <c r="AD8" s="40"/>
     </row>
-    <row r="9" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="A9" s="40"/>
       <c r="B9" s="40"/>
       <c r="C9" s="15">
         <f>C8+$P$3</f>
-        <v>30</v>
-      </c>
-      <c r="D9" s="37">
-        <v>0.4</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D9" s="37"/>
       <c r="E9" s="40"/>
       <c r="F9" s="15">
         <f>F8+$P$3</f>
-        <v>30</v>
-      </c>
-      <c r="G9" s="37">
-        <v>1200</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="G9" s="37"/>
       <c r="H9" s="40"/>
       <c r="I9" s="40"/>
       <c r="J9" s="40"/>
@@ -2619,7 +2607,7 @@
       <c r="AC9" s="40"/>
       <c r="AD9" s="40"/>
     </row>
-    <row r="10" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" outlineLevel="1" x14ac:dyDescent="0.4">
       <c r="A10" s="40"/>
       <c r="B10" s="40"/>
       <c r="C10" s="40"/>
@@ -2650,7 +2638,7 @@
       <c r="AC10" s="40"/>
       <c r="AD10" s="40"/>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A11" s="40"/>
       <c r="B11" s="40"/>
       <c r="C11" s="40"/>
@@ -2680,7 +2668,7 @@
       <c r="AC11" s="40"/>
       <c r="AD11" s="40"/>
     </row>
-    <row r="12" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" ht="16.3" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="40"/>
       <c r="B12" s="40"/>
       <c r="C12" s="40"/>
@@ -2698,11 +2686,11 @@
       <c r="O12" s="40"/>
       <c r="P12" s="40"/>
       <c r="Q12" s="40"/>
-      <c r="R12" s="65" t="str">
+      <c r="R12" s="66" t="str">
         <f>VLOOKUP($C$2,ModelDB[],4,FALSE)</f>
         <v>Glucose</v>
       </c>
-      <c r="S12" s="65"/>
+      <c r="S12" s="66"/>
       <c r="T12" s="40"/>
       <c r="U12" s="28"/>
       <c r="V12" s="28"/>
@@ -2715,7 +2703,7 @@
       <c r="AC12" s="40"/>
       <c r="AD12" s="40"/>
     </row>
-    <row r="13" spans="1:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" ht="30" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="40"/>
       <c r="C13" s="40"/>
       <c r="D13" s="40"/>
@@ -2752,7 +2740,7 @@
       <c r="AC13" s="40"/>
       <c r="AD13" s="40"/>
     </row>
-    <row r="14" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A14" s="40"/>
       <c r="B14" s="45" t="s">
         <v>30</v>
@@ -2780,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="Q14" s="37">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="R14" s="37"/>
       <c r="S14" s="40"/>
@@ -2796,7 +2784,7 @@
       <c r="AC14" s="40"/>
       <c r="AD14" s="40"/>
     </row>
-    <row r="15" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A15" s="40"/>
       <c r="B15" s="40"/>
       <c r="C15" s="15">
@@ -2828,11 +2816,11 @@
       <c r="O15" s="40"/>
       <c r="P15" s="15">
         <f>P14+$N$3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="37"/>
       <c r="R15" s="37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="S15" s="40"/>
       <c r="T15" s="40"/>
@@ -2847,12 +2835,12 @@
       <c r="AC15" s="40"/>
       <c r="AD15" s="40"/>
     </row>
-    <row r="16" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A16" s="40"/>
       <c r="B16" s="40"/>
       <c r="C16" s="15">
         <f>C15+$N$3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D16" s="37">
         <v>100</v>
@@ -2881,12 +2869,10 @@
       <c r="O16" s="40"/>
       <c r="P16" s="15">
         <f>P15+$O$3</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="Q16" s="37"/>
-      <c r="R16" s="37">
-        <v>2</v>
-      </c>
+      <c r="R16" s="37"/>
       <c r="S16" s="40"/>
       <c r="T16" s="40"/>
       <c r="U16" s="28"/>
@@ -2900,16 +2886,14 @@
       <c r="AC16" s="40"/>
       <c r="AD16" s="40"/>
     </row>
-    <row r="17" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="40"/>
       <c r="B17" s="40"/>
       <c r="C17" s="15">
         <f>C16+$O$3</f>
-        <v>20</v>
-      </c>
-      <c r="D17" s="37">
-        <v>120</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D17" s="37"/>
       <c r="E17" s="40"/>
       <c r="F17" s="5"/>
       <c r="G17" s="6"/>
@@ -2925,12 +2909,10 @@
       <c r="O17" s="40"/>
       <c r="P17" s="15">
         <f>P16+$P$3</f>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="Q17" s="38"/>
-      <c r="R17" s="37">
-        <v>4</v>
-      </c>
+      <c r="R17" s="37"/>
       <c r="S17" s="40"/>
       <c r="T17" s="40"/>
       <c r="U17" s="28"/>
@@ -2944,16 +2926,14 @@
       <c r="AC17" s="40"/>
       <c r="AD17" s="40"/>
     </row>
-    <row r="18" spans="1:30" ht="19.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:30" ht="18" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A18" s="40"/>
       <c r="B18" s="40"/>
       <c r="C18" s="15">
         <f>C17+$P$3</f>
-        <v>30</v>
-      </c>
-      <c r="D18" s="37">
-        <v>140</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D18" s="37"/>
       <c r="E18" s="40"/>
       <c r="F18" s="5"/>
       <c r="G18" s="6" t="s">
@@ -2974,11 +2954,11 @@
       </c>
       <c r="Q18" s="50">
         <f>SUM(Q14:Q17)</f>
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="R18" s="51">
         <f>SUMPRODUCT(Input_Array!D4:D7,Input_Array!H4:H7)</f>
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
@@ -2993,7 +2973,7 @@
       <c r="AC18" s="40"/>
       <c r="AD18" s="40"/>
     </row>
-    <row r="19" spans="1:30" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:30" ht="21" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A19" s="40"/>
       <c r="B19" s="40"/>
       <c r="C19" s="40"/>
@@ -3033,7 +3013,7 @@
       <c r="AC19" s="40"/>
       <c r="AD19" s="40"/>
     </row>
-    <row r="20" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="16.3" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="40"/>
       <c r="B20" s="40"/>
       <c r="C20" s="40"/>
@@ -3053,11 +3033,11 @@
       <c r="O20" s="40"/>
       <c r="P20" s="40"/>
       <c r="Q20" s="40"/>
-      <c r="R20" s="65" t="str">
+      <c r="R20" s="66" t="str">
         <f>VLOOKUP($C$2,ModelDB[],5,FALSE)</f>
         <v>(NH4)2SO4</v>
       </c>
-      <c r="S20" s="65"/>
+      <c r="S20" s="66"/>
       <c r="T20" s="40"/>
       <c r="U20" s="28"/>
       <c r="V20" s="28"/>
@@ -3070,7 +3050,7 @@
       <c r="AC20" s="40"/>
       <c r="AD20" s="40"/>
     </row>
-    <row r="21" spans="1:30" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="16.3" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A21" s="40"/>
       <c r="B21" s="40"/>
       <c r="C21" s="40"/>
@@ -3114,7 +3094,7 @@
       <c r="AC21" s="40"/>
       <c r="AD21" s="40"/>
     </row>
-    <row r="22" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A22" s="40"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -3158,16 +3138,16 @@
       <c r="AC22" s="40"/>
       <c r="AD22" s="40"/>
     </row>
-    <row r="23" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A23" s="40"/>
       <c r="B23" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="65" t="str">
+      <c r="C23" s="66" t="str">
         <f>VLOOKUP($C$2,ModelDB[],6,FALSE)</f>
         <v>Ethanol</v>
       </c>
-      <c r="D23" s="65"/>
+      <c r="D23" s="66"/>
       <c r="E23" s="40"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -3183,10 +3163,10 @@
       <c r="O23" s="40"/>
       <c r="P23" s="15">
         <f>P22+$N$3</f>
+        <v>20</v>
+      </c>
+      <c r="Q23" s="37">
         <v>10</v>
-      </c>
-      <c r="Q23" s="37">
-        <v>5</v>
       </c>
       <c r="R23" s="28"/>
       <c r="S23" s="40"/>
@@ -3202,7 +3182,7 @@
       <c r="AC23" s="40"/>
       <c r="AD23" s="40"/>
     </row>
-    <row r="24" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:30" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="40"/>
       <c r="C24" s="40"/>
       <c r="D24" s="40"/>
@@ -3221,11 +3201,9 @@
       <c r="O24" s="40"/>
       <c r="P24" s="15">
         <f>P23+$O$3</f>
-        <v>20</v>
-      </c>
-      <c r="Q24" s="37">
-        <v>5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Q24" s="37"/>
       <c r="R24" s="28"/>
       <c r="S24" s="40"/>
       <c r="T24" s="40"/>
@@ -3240,7 +3218,7 @@
       <c r="AC24" s="40"/>
       <c r="AD24" s="40"/>
     </row>
-    <row r="25" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="40"/>
       <c r="B25" s="40"/>
       <c r="C25" s="40"/>
@@ -3260,11 +3238,9 @@
       <c r="O25" s="40"/>
       <c r="P25" s="53">
         <f>P24+$P$3</f>
-        <v>30</v>
-      </c>
-      <c r="Q25" s="38">
-        <v>5</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="Q25" s="38"/>
       <c r="R25" s="28"/>
       <c r="S25" s="40"/>
       <c r="T25" s="40"/>
@@ -3279,7 +3255,7 @@
       <c r="AC25" s="40"/>
       <c r="AD25" s="40"/>
     </row>
-    <row r="26" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="40"/>
       <c r="B26" s="40"/>
       <c r="C26" s="40"/>
@@ -3302,7 +3278,7 @@
       </c>
       <c r="Q26" s="50">
         <f>SUM(Q22:Q25)</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="R26" s="28"/>
       <c r="S26" s="40"/>
@@ -3318,7 +3294,7 @@
       <c r="AC26" s="40"/>
       <c r="AD26" s="40"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A27" s="40"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -3352,7 +3328,7 @@
       <c r="AC27" s="40"/>
       <c r="AD27" s="40"/>
     </row>
-    <row r="28" spans="1:30" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:30" ht="18.45" x14ac:dyDescent="0.5">
       <c r="A28" s="40"/>
       <c r="B28" s="44"/>
       <c r="C28" s="40"/>
@@ -3386,7 +3362,7 @@
       <c r="AC28" s="40"/>
       <c r="AD28" s="40"/>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A29" s="40"/>
       <c r="B29" s="40"/>
       <c r="C29" s="40"/>
@@ -3420,7 +3396,7 @@
       <c r="AC29" s="40"/>
       <c r="AD29" s="40"/>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A30" s="40"/>
       <c r="B30" s="40"/>
       <c r="C30" s="40"/>
@@ -3450,7 +3426,7 @@
       <c r="AC30" s="40"/>
       <c r="AD30" s="40"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A31" s="40"/>
       <c r="B31" s="40"/>
       <c r="C31" s="40"/>
@@ -3482,7 +3458,7 @@
       <c r="AC31" s="40"/>
       <c r="AD31" s="40"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A32" s="40"/>
       <c r="B32" s="40"/>
       <c r="C32" s="40"/>
@@ -3514,7 +3490,7 @@
       <c r="AC32" s="40"/>
       <c r="AD32" s="40"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A33" s="40"/>
       <c r="B33" s="40"/>
       <c r="C33" s="40"/>
@@ -3546,7 +3522,7 @@
       <c r="AC33" s="40"/>
       <c r="AD33" s="40"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A34" s="40"/>
       <c r="B34" s="40"/>
       <c r="C34" s="40"/>
@@ -3578,7 +3554,7 @@
       <c r="AC34" s="40"/>
       <c r="AD34" s="40"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A35" s="40"/>
       <c r="B35" s="40"/>
       <c r="C35" s="40"/>
@@ -3610,7 +3586,7 @@
       <c r="AC35" s="40"/>
       <c r="AD35" s="40"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A36" s="40"/>
       <c r="B36" s="40"/>
       <c r="C36" s="40"/>
@@ -3642,7 +3618,7 @@
       <c r="AC36" s="40"/>
       <c r="AD36" s="40"/>
     </row>
-    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A37" s="40"/>
       <c r="B37" s="40"/>
       <c r="C37" s="40"/>
@@ -3674,7 +3650,7 @@
       <c r="AC37" s="40"/>
       <c r="AD37" s="40"/>
     </row>
-    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:30" x14ac:dyDescent="0.4">
       <c r="U38" s="40"/>
       <c r="V38" s="40"/>
       <c r="W38" s="40"/>
@@ -3686,7 +3662,7 @@
       <c r="AC38" s="40"/>
       <c r="AD38" s="40"/>
     </row>
-    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.4">
       <c r="U39" s="40"/>
       <c r="V39" s="40"/>
       <c r="W39" s="40"/>
@@ -3728,33 +3704,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E029EF7D-A343-4D00-BDC4-8E8C5E795D32}">
   <dimension ref="A1:AA42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="21" max="21" width="27.140625" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" customWidth="1"/>
-    <col min="24" max="24" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="29.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3828125" customWidth="1"/>
+    <col min="21" max="21" width="27.15234375" customWidth="1"/>
+    <col min="22" max="22" width="24.3828125" customWidth="1"/>
+    <col min="24" max="24" width="16.84375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="29.15234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>68</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>25</v>
       </c>
@@ -3807,7 +3783,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -3817,7 +3793,7 @@
       </c>
       <c r="C4" cm="1">
         <f t="array" ref="C4:C7">Hübsch!Q14:Q17</f>
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f>Hübsch!R14</f>
@@ -3837,7 +3813,7 @@
       </c>
       <c r="H4">
         <f>Hübsch!N3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I4">
         <f>Hübsch!$G$19</f>
@@ -3867,7 +3843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -3880,11 +3856,11 @@
       </c>
       <c r="D5">
         <f>Hübsch!R15</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E5">
         <f>Hübsch!Q23</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5">
         <f>Hübsch!G7</f>
@@ -3892,11 +3868,11 @@
       </c>
       <c r="G5">
         <f>Hübsch!D7</f>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="H5">
         <f>Hübsch!O3</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="I5">
         <f>Hübsch!$G$19</f>
@@ -3917,36 +3893,36 @@
       </c>
       <c r="Q5" s="64"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6">
         <f>Hübsch!D17</f>
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
         <f>Hübsch!R16</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <f>Hübsch!Q24</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <f>Hübsch!G8</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <f>Hübsch!D8</f>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <f>Hübsch!P3</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <f>Hübsch!$G$19</f>
@@ -3967,36 +3943,36 @@
       </c>
       <c r="Q6" s="64"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A7" s="60">
         <v>4</v>
       </c>
       <c r="B7">
         <f>Hübsch!D18</f>
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
         <f>Hübsch!R17</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <f>Hübsch!Q25</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f>Hübsch!G9</f>
-        <v>1200</v>
+        <v>0</v>
       </c>
       <c r="G7">
         <f>Hübsch!D9</f>
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <f>Hübsch!Q3</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <f>Hübsch!$G$19</f>
@@ -4017,22 +3993,22 @@
       </c>
       <c r="Q7" s="64"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -4049,7 +4025,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B14">
         <v>0.7</v>
       </c>
@@ -4063,12 +4039,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -4145,7 +4121,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A23">
         <f>VLOOKUP(Hübsch!$C$2,ModelDB[#All],7,FALSE)</f>
         <v>0.46209812037329684</v>
@@ -4246,12 +4222,12 @@
         <v>nicht wachstumsassoziierte Ethanolbildung mit hohem Ks --&gt; höhere Biomassegehalte bei niedrigen Substrat 1 konz.</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A37">
         <v>1</v>
       </c>
@@ -4334,7 +4310,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.4">
       <c r="A38" s="2" t="s">
         <v>2</v>
       </c>
@@ -4417,7 +4393,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="63" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
         <v>1</v>
       </c>
@@ -4464,7 +4440,7 @@
       <c r="O39" s="2">
         <v>1</v>
       </c>
-      <c r="P39" s="69">
+      <c r="P39" s="65">
         <v>0.5</v>
       </c>
       <c r="Q39" s="2">
@@ -4500,7 +4476,7 @@
       </c>
       <c r="AA39" s="2"/>
     </row>
-    <row r="40" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
         <v>2</v>
       </c>
@@ -4580,7 +4556,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="58.3" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -4662,7 +4638,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="43.75" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
         <v>4</v>
       </c>
@@ -4755,9 +4731,9 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>28</v>
       </c>

</xml_diff>